<commit_message>
Changed Wenglor relative height uncertainty values
Decreased Wenglor relative height uncertainty from +/- 1 cm to +/- 1
mm.  Original value was too large.  The relative height uncertainty is
related to the positioning within the Wenglor array, which was
determined to high precision in the lab prior to deployment of the
array.  More of the height uncertainty (which is captured from the
distance sensor) is due to the position of the array relative to the
ground.
</commit_message>
<xml_diff>
--- a/Metadata/InstrumentMetadata_Jericoacoara.xlsx
+++ b/Metadata/InstrumentMetadata_Jericoacoara.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="53">
   <si>
     <t>Site</t>
   </si>
@@ -245,8 +245,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="645">
+  <cellStyleXfs count="647">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -905,7 +907,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="645">
+  <cellStyles count="647">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1228,6 +1230,7 @@
     <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1550,6 +1553,7 @@
     <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1882,9 +1886,9 @@
   <dimension ref="A1:O114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="A1:O114"/>
+      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1974,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J2" t="s">
         <v>16</v>
@@ -2021,10 +2025,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
       </c>
       <c r="K3" s="5">
         <v>-0.05</v>
@@ -2068,7 +2072,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J4" t="s">
         <v>16</v>
@@ -2115,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>16</v>
@@ -2162,7 +2166,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J6" t="s">
         <v>14</v>
@@ -2209,10 +2213,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="K7" s="5">
         <v>-0.05</v>
@@ -2256,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J8" t="s">
         <v>14</v>
@@ -2303,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>14</v>
@@ -2350,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>25</v>
@@ -2397,7 +2401,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>25</v>
@@ -2444,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>26</v>
@@ -2491,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>26</v>
@@ -3525,7 +3529,7 @@
         <v>-0.33500000000000002</v>
       </c>
       <c r="I35" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J35" t="s">
         <v>16</v>
@@ -3572,7 +3576,7 @@
         <v>-0.33500000000000002</v>
       </c>
       <c r="I36" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J36" t="s">
         <v>16</v>
@@ -3619,7 +3623,7 @@
         <v>-0.33500000000000002</v>
       </c>
       <c r="I37" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J37" t="s">
         <v>16</v>
@@ -3666,7 +3670,7 @@
         <v>-0.33500000000000002</v>
       </c>
       <c r="I38" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J38" t="s">
         <v>16</v>
@@ -3713,7 +3717,7 @@
         <v>-0.33500000000000002</v>
       </c>
       <c r="I39" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J39" t="s">
         <v>16</v>
@@ -3760,7 +3764,7 @@
         <v>-0.33500000000000002</v>
       </c>
       <c r="I40" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J40" t="s">
         <v>16</v>
@@ -3807,7 +3811,7 @@
         <v>-0.33500000000000002</v>
       </c>
       <c r="I41" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J41" t="s">
         <v>16</v>
@@ -3854,7 +3858,7 @@
         <v>-4.0000000000000036E-3</v>
       </c>
       <c r="I42" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J42" t="s">
         <v>16</v>
@@ -3901,7 +3905,7 @@
         <v>-4.0000000000000036E-3</v>
       </c>
       <c r="I43" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J43" t="s">
         <v>16</v>
@@ -3948,7 +3952,7 @@
         <v>-4.0000000000000036E-3</v>
       </c>
       <c r="I44" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J44" t="s">
         <v>16</v>
@@ -3995,7 +3999,7 @@
         <v>-0.26500000000000001</v>
       </c>
       <c r="I45" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J45" t="s">
         <v>16</v>
@@ -4042,7 +4046,7 @@
         <v>-0.26500000000000001</v>
       </c>
       <c r="I46" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J46" t="s">
         <v>16</v>
@@ -4089,7 +4093,7 @@
         <v>-0.26500000000000001</v>
       </c>
       <c r="I47" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J47" t="s">
         <v>16</v>
@@ -4136,7 +4140,7 @@
         <v>-0.26500000000000001</v>
       </c>
       <c r="I48" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J48" t="s">
         <v>16</v>
@@ -4183,7 +4187,7 @@
         <v>-0.26500000000000001</v>
       </c>
       <c r="I49" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J49" t="s">
         <v>16</v>
@@ -4230,7 +4234,7 @@
         <v>-0.26500000000000001</v>
       </c>
       <c r="I50" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J50" t="s">
         <v>16</v>
@@ -4277,7 +4281,7 @@
         <v>-0.26500000000000001</v>
       </c>
       <c r="I51" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J51" t="s">
         <v>16</v>
@@ -4324,7 +4328,7 @@
         <v>-0.155</v>
       </c>
       <c r="I52" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J52" t="s">
         <v>16</v>
@@ -4371,7 +4375,7 @@
         <v>-0.155</v>
       </c>
       <c r="I53" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J53" t="s">
         <v>16</v>
@@ -4418,7 +4422,7 @@
         <v>-0.155</v>
       </c>
       <c r="I54" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J54" t="s">
         <v>16</v>
@@ -4465,7 +4469,7 @@
         <v>-0.38500000000000001</v>
       </c>
       <c r="I55" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J55" t="s">
         <v>16</v>
@@ -4512,7 +4516,7 @@
         <v>-0.38500000000000001</v>
       </c>
       <c r="I56" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J56" t="s">
         <v>16</v>
@@ -4559,7 +4563,7 @@
         <v>-0.22500000000000001</v>
       </c>
       <c r="I57" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J57" t="s">
         <v>14</v>
@@ -4606,7 +4610,7 @@
         <v>-0.22500000000000001</v>
       </c>
       <c r="I58" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J58" t="s">
         <v>14</v>
@@ -4653,7 +4657,7 @@
         <v>-0.22500000000000001</v>
       </c>
       <c r="I59" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J59" t="s">
         <v>14</v>
@@ -4700,7 +4704,7 @@
         <v>-0.22500000000000001</v>
       </c>
       <c r="I60" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J60" t="s">
         <v>14</v>
@@ -4747,7 +4751,7 @@
         <v>-0.22500000000000001</v>
       </c>
       <c r="I61" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J61" t="s">
         <v>14</v>
@@ -4794,7 +4798,7 @@
         <v>-0.22500000000000001</v>
       </c>
       <c r="I62" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J62" t="s">
         <v>14</v>
@@ -4841,7 +4845,7 @@
         <v>-0.22500000000000001</v>
       </c>
       <c r="I63" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J63" t="s">
         <v>14</v>
@@ -4888,7 +4892,7 @@
         <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I64" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J64" t="s">
         <v>26</v>
@@ -4935,7 +4939,7 @@
         <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I65" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J65" t="s">
         <v>26</v>
@@ -4982,7 +4986,7 @@
         <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I66" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J66" t="s">
         <v>26</v>
@@ -5029,7 +5033,7 @@
         <v>-0.155</v>
       </c>
       <c r="I67" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J67" t="s">
         <v>14</v>
@@ -5076,7 +5080,7 @@
         <v>-0.155</v>
       </c>
       <c r="I68" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J68" t="s">
         <v>14</v>
@@ -5123,7 +5127,7 @@
         <v>-0.155</v>
       </c>
       <c r="I69" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J69" t="s">
         <v>14</v>
@@ -5170,7 +5174,7 @@
         <v>-0.155</v>
       </c>
       <c r="I70" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J70" t="s">
         <v>14</v>
@@ -5217,7 +5221,7 @@
         <v>-0.155</v>
       </c>
       <c r="I71" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J71" t="s">
         <v>14</v>
@@ -5264,7 +5268,7 @@
         <v>-0.155</v>
       </c>
       <c r="I72" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J72" t="s">
         <v>14</v>
@@ -5311,7 +5315,7 @@
         <v>-0.155</v>
       </c>
       <c r="I73" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J73" t="s">
         <v>14</v>
@@ -5358,7 +5362,7 @@
         <v>8.0999999999999989E-2</v>
       </c>
       <c r="I74" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J74" t="s">
         <v>26</v>
@@ -5405,7 +5409,7 @@
         <v>8.0999999999999989E-2</v>
       </c>
       <c r="I75" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J75" t="s">
         <v>26</v>
@@ -5452,7 +5456,7 @@
         <v>8.0999999999999989E-2</v>
       </c>
       <c r="I76" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J76" t="s">
         <v>26</v>
@@ -5499,7 +5503,7 @@
         <v>-0.32500000000000001</v>
       </c>
       <c r="I77" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J77" t="s">
         <v>14</v>
@@ -5546,7 +5550,7 @@
         <v>-0.32500000000000001</v>
       </c>
       <c r="I78" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J78" t="s">
         <v>14</v>
@@ -5593,7 +5597,7 @@
         <v>-0.32500000000000001</v>
       </c>
       <c r="I79" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J79" t="s">
         <v>14</v>
@@ -5640,7 +5644,7 @@
         <v>-0.32500000000000001</v>
       </c>
       <c r="I80" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J80" t="s">
         <v>14</v>
@@ -5687,7 +5691,7 @@
         <v>-0.32500000000000001</v>
       </c>
       <c r="I81" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J81" t="s">
         <v>14</v>
@@ -5734,7 +5738,7 @@
         <v>-0.32500000000000001</v>
       </c>
       <c r="I82" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J82" t="s">
         <v>14</v>
@@ -5781,7 +5785,7 @@
         <v>-0.32500000000000001</v>
       </c>
       <c r="I83" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J83" t="s">
         <v>14</v>
@@ -5828,7 +5832,7 @@
         <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I84" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J84" t="s">
         <v>26</v>
@@ -5875,7 +5879,7 @@
         <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I85" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J85" t="s">
         <v>26</v>
@@ -5922,7 +5926,7 @@
         <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I86" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J86" t="s">
         <v>26</v>
@@ -5969,7 +5973,7 @@
         <v>-0.28500000000000003</v>
       </c>
       <c r="I87" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J87" t="s">
         <v>14</v>
@@ -6016,7 +6020,7 @@
         <v>-0.28500000000000003</v>
       </c>
       <c r="I88" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J88" t="s">
         <v>14</v>
@@ -6063,7 +6067,7 @@
         <v>-0.28500000000000003</v>
       </c>
       <c r="I89" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J89" t="s">
         <v>14</v>
@@ -6110,7 +6114,7 @@
         <v>-0.28500000000000003</v>
       </c>
       <c r="I90" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J90" t="s">
         <v>14</v>
@@ -6157,7 +6161,7 @@
         <v>-0.28500000000000003</v>
       </c>
       <c r="I91" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J91" t="s">
         <v>14</v>
@@ -6204,7 +6208,7 @@
         <v>-0.28500000000000003</v>
       </c>
       <c r="I92" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J92" t="s">
         <v>14</v>
@@ -6251,7 +6255,7 @@
         <v>-0.28500000000000003</v>
       </c>
       <c r="I93" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J93" t="s">
         <v>14</v>
@@ -6298,7 +6302,7 @@
         <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I94" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J94" t="s">
         <v>26</v>
@@ -6345,7 +6349,7 @@
         <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I95" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J95" t="s">
         <v>26</v>
@@ -6392,7 +6396,7 @@
         <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I96" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J96" t="s">
         <v>26</v>
@@ -6439,7 +6443,7 @@
         <v>-0.155</v>
       </c>
       <c r="I97" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J97" t="s">
         <v>16</v>
@@ -6486,7 +6490,7 @@
         <v>-0.155</v>
       </c>
       <c r="I98" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J98" t="s">
         <v>16</v>
@@ -6533,7 +6537,7 @@
         <v>-0.155</v>
       </c>
       <c r="I99" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J99" t="s">
         <v>16</v>
@@ -6580,7 +6584,7 @@
         <v>-0.155</v>
       </c>
       <c r="I100" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J100" t="s">
         <v>16</v>
@@ -6627,7 +6631,7 @@
         <v>-0.155</v>
       </c>
       <c r="I101" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J101" t="s">
         <v>16</v>
@@ -6674,7 +6678,7 @@
         <v>-0.155</v>
       </c>
       <c r="I102" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J102" t="s">
         <v>16</v>
@@ -6721,7 +6725,7 @@
         <v>-0.155</v>
       </c>
       <c r="I103" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J103" t="s">
         <v>16</v>
@@ -6768,7 +6772,7 @@
         <v>-0.155</v>
       </c>
       <c r="I104" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J104" t="s">
         <v>16</v>
@@ -6815,7 +6819,7 @@
         <v>-0.155</v>
       </c>
       <c r="I105" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J105" t="s">
         <v>16</v>
@@ -6862,7 +6866,7 @@
         <v>-0.155</v>
       </c>
       <c r="I106" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J106" t="s">
         <v>16</v>
@@ -6909,7 +6913,7 @@
         <v>-0.38500000000000001</v>
       </c>
       <c r="I107" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J107" t="s">
         <v>16</v>
@@ -6956,7 +6960,7 @@
         <v>-0.38500000000000001</v>
       </c>
       <c r="I108" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J108" t="s">
         <v>16</v>
@@ -7003,7 +7007,7 @@
         <v>-0.38500000000000001</v>
       </c>
       <c r="I109" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J109" t="s">
         <v>16</v>
@@ -7050,7 +7054,7 @@
         <v>-0.38500000000000001</v>
       </c>
       <c r="I110" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J110" t="s">
         <v>16</v>
@@ -7097,7 +7101,7 @@
         <v>-0.38500000000000001</v>
       </c>
       <c r="I111" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J111" t="s">
         <v>16</v>
@@ -7144,7 +7148,7 @@
         <v>-0.155</v>
       </c>
       <c r="I112" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J112" t="s">
         <v>16</v>
@@ -7191,7 +7195,7 @@
         <v>-0.155</v>
       </c>
       <c r="I113" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J113" t="s">
         <v>16</v>
@@ -7238,7 +7242,7 @@
         <v>-0.155</v>
       </c>
       <c r="I114" s="4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J114" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Restored certain time intervals previously removed
Time intervals previously removed had too few Wenglor heights.  But
decided it would be better to keep these in the processing, then filter
them out when plotting later.
</commit_message>
<xml_diff>
--- a/Metadata/InstrumentMetadata_Jericoacoara.xlsx
+++ b/Metadata/InstrumentMetadata_Jericoacoara.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="37320" windowHeight="10860" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="53">
   <si>
     <t>Site</t>
   </si>
@@ -1883,12 +1883,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O106"/>
+  <dimension ref="A1:O114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C106" sqref="C106"/>
+      <selection pane="bottomLeft" activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6887,6 +6887,382 @@
         <v>52</v>
       </c>
     </row>
+    <row r="107" spans="1:15">
+      <c r="A107" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B107" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C107" s="3">
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="D107" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F107" t="s">
+        <v>19</v>
+      </c>
+      <c r="G107" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="H107" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="I107" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J107" t="s">
+        <v>16</v>
+      </c>
+      <c r="K107" s="4">
+        <v>0</v>
+      </c>
+      <c r="L107" s="4">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="M107" s="4">
+        <v>0</v>
+      </c>
+      <c r="N107" s="4">
+        <v>1</v>
+      </c>
+      <c r="O107" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15">
+      <c r="A108" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B108" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C108" s="3">
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="D108" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F108" t="s">
+        <v>20</v>
+      </c>
+      <c r="G108" s="4">
+        <v>-4.0000000000000036E-3</v>
+      </c>
+      <c r="H108" s="4">
+        <v>-4.0000000000000036E-3</v>
+      </c>
+      <c r="I108" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J108" t="s">
+        <v>16</v>
+      </c>
+      <c r="K108" s="4">
+        <v>0</v>
+      </c>
+      <c r="L108" s="4">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="M108" s="4">
+        <v>0</v>
+      </c>
+      <c r="N108" s="4">
+        <v>0</v>
+      </c>
+      <c r="O108" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15">
+      <c r="A109" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B109" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C109" s="3">
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="D109" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F109" t="s">
+        <v>21</v>
+      </c>
+      <c r="G109" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="H109" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="I109" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J109" t="s">
+        <v>26</v>
+      </c>
+      <c r="K109" s="4">
+        <v>0</v>
+      </c>
+      <c r="L109" s="4">
+        <v>-0.496</v>
+      </c>
+      <c r="M109" s="4">
+        <v>0</v>
+      </c>
+      <c r="N109" s="4">
+        <v>0</v>
+      </c>
+      <c r="O109" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15">
+      <c r="A110" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B110" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C110" s="3">
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="D110" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F110" t="s">
+        <v>22</v>
+      </c>
+      <c r="G110" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="H110" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="I110" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J110" t="s">
+        <v>26</v>
+      </c>
+      <c r="K110" s="4">
+        <v>0</v>
+      </c>
+      <c r="L110" s="4">
+        <v>-0.66500000000000004</v>
+      </c>
+      <c r="M110" s="4">
+        <v>0</v>
+      </c>
+      <c r="N110" s="4">
+        <v>0</v>
+      </c>
+      <c r="O110" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15">
+      <c r="A111" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C111" s="3">
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="D111" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F111" t="s">
+        <v>23</v>
+      </c>
+      <c r="G111" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="H111" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="I111" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J111" t="s">
+        <v>26</v>
+      </c>
+      <c r="K111" s="4">
+        <v>0</v>
+      </c>
+      <c r="L111" s="4">
+        <v>-0.92900000000000005</v>
+      </c>
+      <c r="M111" s="4">
+        <v>0</v>
+      </c>
+      <c r="N111" s="4">
+        <v>0</v>
+      </c>
+      <c r="O111" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15">
+      <c r="A112" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B112" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C112" s="3">
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="D112" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F112" t="s">
+        <v>24</v>
+      </c>
+      <c r="G112" s="4">
+        <v>8.0999999999999989E-2</v>
+      </c>
+      <c r="H112" s="4">
+        <v>8.0999999999999989E-2</v>
+      </c>
+      <c r="I112" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J112" t="s">
+        <v>26</v>
+      </c>
+      <c r="K112" s="4">
+        <v>0</v>
+      </c>
+      <c r="L112" s="4">
+        <v>-0.92900000000000005</v>
+      </c>
+      <c r="M112" s="4">
+        <v>0</v>
+      </c>
+      <c r="N112" s="4">
+        <v>0</v>
+      </c>
+      <c r="O112" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15">
+      <c r="A113" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B113" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C113" s="3">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D113" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F113" t="s">
+        <v>17</v>
+      </c>
+      <c r="G113" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="H113" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="I113" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J113" t="s">
+        <v>16</v>
+      </c>
+      <c r="K113" s="4">
+        <v>0</v>
+      </c>
+      <c r="L113" s="4">
+        <v>0.251</v>
+      </c>
+      <c r="M113" s="4">
+        <v>0</v>
+      </c>
+      <c r="N113" s="4">
+        <v>1</v>
+      </c>
+      <c r="O113" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15">
+      <c r="A114" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B114" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C114" s="3">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D114" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F114" t="s">
+        <v>18</v>
+      </c>
+      <c r="G114" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="H114" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="I114" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J114" t="s">
+        <v>16</v>
+      </c>
+      <c r="K114" s="4">
+        <v>0</v>
+      </c>
+      <c r="L114" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M114" s="4">
+        <v>0</v>
+      </c>
+      <c r="N114" s="4">
+        <v>1</v>
+      </c>
+      <c r="O114" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:O114">
     <sortCondition ref="B2:B114"/>

</xml_diff>

<commit_message>
Changed range of data for analysis
Removed some Wenglor time intervals disrupted by rain drops
</commit_message>
<xml_diff>
--- a/Metadata/InstrumentMetadata_Jericoacoara.xlsx
+++ b/Metadata/InstrumentMetadata_Jericoacoara.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raleighmartin/GitHub/Jericoacoara2014/Metadata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13760" tabRatio="500"/>
+    <workbookView xWindow="27280" yWindow="4100" windowWidth="25120" windowHeight="13760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="53">
   <si>
     <t>Site</t>
   </si>
@@ -1558,6 +1566,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1883,15 +1896,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:O106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E93" sqref="E93"/>
+      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
@@ -1905,7 +1918,7 @@
     <col min="15" max="15" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1952,7 +1965,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1999,7 +2012,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -2046,7 +2059,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -2093,7 +2106,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -2140,7 +2153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -2187,7 +2200,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -2234,7 +2247,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -2281,7 +2294,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -2328,7 +2341,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -2375,7 +2388,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -2422,7 +2435,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2469,7 +2482,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -2516,7 +2529,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -2563,7 +2576,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -2610,7 +2623,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -2657,7 +2670,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -2704,7 +2717,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -2751,7 +2764,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -2798,7 +2811,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
@@ -2845,7 +2858,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
@@ -2892,7 +2905,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
@@ -2939,7 +2952,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
@@ -2986,7 +2999,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
@@ -3033,7 +3046,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -3080,7 +3093,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
@@ -3127,7 +3140,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>13</v>
       </c>
@@ -3174,7 +3187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>13</v>
       </c>
@@ -3221,7 +3234,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>13</v>
       </c>
@@ -3268,7 +3281,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
@@ -3315,7 +3328,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>13</v>
       </c>
@@ -3362,7 +3375,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>13</v>
       </c>
@@ -3409,7 +3422,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>13</v>
       </c>
@@ -3456,7 +3469,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>13</v>
       </c>
@@ -3503,7 +3516,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>13</v>
       </c>
@@ -3550,7 +3563,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>13</v>
       </c>
@@ -3597,7 +3610,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>13</v>
       </c>
@@ -3644,7 +3657,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>13</v>
       </c>
@@ -3691,7 +3704,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>13</v>
       </c>
@@ -3738,7 +3751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>13</v>
       </c>
@@ -3785,7 +3798,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>13</v>
       </c>
@@ -3832,7 +3845,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>13</v>
       </c>
@@ -3879,7 +3892,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>13</v>
       </c>
@@ -3926,7 +3939,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>13</v>
       </c>
@@ -3973,7 +3986,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>13</v>
       </c>
@@ -4020,7 +4033,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>13</v>
       </c>
@@ -4067,7 +4080,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>13</v>
       </c>
@@ -4114,7 +4127,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>13</v>
       </c>
@@ -4161,7 +4174,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>13</v>
       </c>
@@ -4208,7 +4221,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>13</v>
       </c>
@@ -4255,7 +4268,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>13</v>
       </c>
@@ -4302,7 +4315,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>13</v>
       </c>
@@ -4349,7 +4362,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>13</v>
       </c>
@@ -4396,7 +4409,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>13</v>
       </c>
@@ -4443,7 +4456,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>13</v>
       </c>
@@ -4490,7 +4503,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>13</v>
       </c>
@@ -4537,7 +4550,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>13</v>
       </c>
@@ -4584,7 +4597,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>13</v>
       </c>
@@ -4631,7 +4644,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>13</v>
       </c>
@@ -4678,7 +4691,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>13</v>
       </c>
@@ -4725,7 +4738,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>13</v>
       </c>
@@ -4772,7 +4785,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>13</v>
       </c>
@@ -4819,7 +4832,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>13</v>
       </c>
@@ -4866,7 +4879,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>13</v>
       </c>
@@ -4913,7 +4926,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>13</v>
       </c>
@@ -4960,7 +4973,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>13</v>
       </c>
@@ -5007,7 +5020,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>13</v>
       </c>
@@ -5054,7 +5067,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>13</v>
       </c>
@@ -5101,7 +5114,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>13</v>
       </c>
@@ -5148,7 +5161,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>13</v>
       </c>
@@ -5195,7 +5208,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>13</v>
       </c>
@@ -5242,7 +5255,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>13</v>
       </c>
@@ -5250,34 +5263,34 @@
         <v>41961</v>
       </c>
       <c r="C72" s="3">
-        <v>0.27083333333333298</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="D72" s="3">
-        <v>0.52430555555555602</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F72" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G72" s="4">
-        <v>-4.0000000000000036E-3</v>
+        <v>0</v>
       </c>
       <c r="H72" s="4">
-        <v>-4.0000000000000036E-3</v>
+        <v>0</v>
       </c>
       <c r="I72" s="4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J72" t="s">
         <v>16</v>
       </c>
-      <c r="K72" s="4">
-        <v>0</v>
+      <c r="K72" s="5">
+        <v>-0.05</v>
       </c>
       <c r="L72" s="4">
-        <v>-7.9000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="M72" s="4">
         <v>0</v>
@@ -5286,10 +5299,10 @@
         <v>0</v>
       </c>
       <c r="O72" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>13</v>
       </c>
@@ -5297,34 +5310,34 @@
         <v>41961</v>
       </c>
       <c r="C73" s="3">
-        <v>0.27083333333333298</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="D73" s="3">
-        <v>0.52430555555555602</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F73" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G73" s="4">
-        <v>-0.155</v>
+        <v>0</v>
       </c>
       <c r="H73" s="4">
-        <v>-0.155</v>
+        <v>0</v>
       </c>
       <c r="I73" s="4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J73" t="s">
-        <v>16</v>
-      </c>
-      <c r="K73" s="4">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="K73" s="5">
+        <v>-0.125</v>
       </c>
       <c r="L73" s="4">
-        <v>-7.9000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="M73" s="4">
         <v>0</v>
@@ -5333,10 +5346,10 @@
         <v>0</v>
       </c>
       <c r="O73" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>13</v>
       </c>
@@ -5344,34 +5357,34 @@
         <v>41961</v>
       </c>
       <c r="C74" s="3">
-        <v>0.27083333333333298</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="D74" s="3">
-        <v>0.52430555555555602</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F74" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G74" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="H74" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="I74" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J74" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="K74" s="4">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="L74" s="4">
-        <v>-0.66500000000000004</v>
+        <v>-0.73</v>
       </c>
       <c r="M74" s="4">
         <v>0</v>
@@ -5379,11 +5392,11 @@
       <c r="N74" s="4">
         <v>0</v>
       </c>
-      <c r="O74" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15">
+      <c r="O74" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>13</v>
       </c>
@@ -5391,34 +5404,34 @@
         <v>41961</v>
       </c>
       <c r="C75" s="3">
-        <v>0.27083333333333298</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="D75" s="3">
-        <v>0.52430555555555602</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F75" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G75" s="4">
-        <v>8.0999999999999989E-2</v>
+        <v>0</v>
       </c>
       <c r="H75" s="4">
-        <v>8.0999999999999989E-2</v>
+        <v>0</v>
       </c>
       <c r="I75" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J75" t="s">
+        <v>0</v>
+      </c>
+      <c r="J75" s="4" t="s">
         <v>26</v>
       </c>
       <c r="K75" s="4">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="L75" s="4">
-        <v>-0.92900000000000005</v>
+        <v>-0.73</v>
       </c>
       <c r="M75" s="4">
         <v>0</v>
@@ -5426,11 +5439,11 @@
       <c r="N75" s="4">
         <v>0</v>
       </c>
-      <c r="O75" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15">
+      <c r="O75" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>13</v>
       </c>
@@ -5438,34 +5451,34 @@
         <v>41961</v>
       </c>
       <c r="C76" s="3">
-        <v>0.27083333333333298</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="D76" s="3">
-        <v>0.52430555555555602</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F76" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G76" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="H76" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="I76" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J76" t="s">
-        <v>26</v>
+        <v>0.01</v>
+      </c>
+      <c r="J76" s="4">
+        <v>0</v>
       </c>
       <c r="K76" s="4">
         <v>0</v>
       </c>
       <c r="L76" s="4">
-        <v>-0.496</v>
+        <v>0</v>
       </c>
       <c r="M76" s="4">
         <v>0</v>
@@ -5473,11 +5486,11 @@
       <c r="N76" s="4">
         <v>0</v>
       </c>
-      <c r="O76" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15">
+      <c r="O76" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>13</v>
       </c>
@@ -5485,46 +5498,46 @@
         <v>41961</v>
       </c>
       <c r="C77" s="3">
-        <v>0.27083333333333298</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="D77" s="3">
-        <v>0.52430555555555602</v>
+        <v>0.47569444444444442</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F77" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G77" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="H77" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="I77" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J77" t="s">
-        <v>26</v>
+        <v>0.01</v>
+      </c>
+      <c r="J77" s="4">
+        <v>0</v>
       </c>
       <c r="K77" s="4">
         <v>0</v>
       </c>
       <c r="L77" s="4">
-        <v>-0.92900000000000005</v>
+        <v>0</v>
       </c>
       <c r="M77" s="4">
         <v>0</v>
       </c>
       <c r="N77" s="4">
-        <v>0</v>
-      </c>
-      <c r="O77" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15">
+        <v>1</v>
+      </c>
+      <c r="O77" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>13</v>
       </c>
@@ -5532,34 +5545,34 @@
         <v>41961</v>
       </c>
       <c r="C78" s="3">
-        <v>0.27083333333333298</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="D78" s="3">
-        <v>0.52430555555555602</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F78" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G78" s="4">
-        <v>-0.155</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="H78" s="4">
-        <v>-0.155</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="I78" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J78" t="s">
-        <v>16</v>
+        <v>0.01</v>
+      </c>
+      <c r="J78" s="4">
+        <v>0</v>
       </c>
       <c r="K78" s="4">
         <v>0</v>
       </c>
       <c r="L78" s="4">
-        <v>8.2000000000000003E-2</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="M78" s="4">
         <v>0</v>
@@ -5567,11 +5580,11 @@
       <c r="N78" s="4">
         <v>0</v>
       </c>
-      <c r="O78" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15">
+      <c r="O78" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>13</v>
       </c>
@@ -5585,28 +5598,28 @@
         <v>0.52430555555555558</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F79" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G79" s="4">
-        <v>0</v>
+        <v>1.7809999999999999</v>
       </c>
       <c r="H79" s="4">
-        <v>0</v>
+        <v>1.7809999999999999</v>
       </c>
       <c r="I79" s="4">
-        <v>0</v>
-      </c>
-      <c r="J79" t="s">
-        <v>16</v>
-      </c>
-      <c r="K79" s="5">
-        <v>-0.05</v>
+        <v>0.01</v>
+      </c>
+      <c r="J79" s="4">
+        <v>0</v>
+      </c>
+      <c r="K79" s="4">
+        <v>0</v>
       </c>
       <c r="L79" s="4">
-        <v>0</v>
+        <v>-0.73</v>
       </c>
       <c r="M79" s="4">
         <v>0</v>
@@ -5615,10 +5628,10 @@
         <v>0</v>
       </c>
       <c r="O79" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>13</v>
       </c>
@@ -5632,10 +5645,10 @@
         <v>0.52430555555555558</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F80" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G80" s="4">
         <v>0</v>
@@ -5646,11 +5659,11 @@
       <c r="I80" s="4">
         <v>0</v>
       </c>
-      <c r="J80" t="s">
-        <v>14</v>
-      </c>
-      <c r="K80" s="5">
-        <v>-0.125</v>
+      <c r="J80" s="4">
+        <v>0</v>
+      </c>
+      <c r="K80" s="4">
+        <v>0</v>
       </c>
       <c r="L80" s="4">
         <v>0</v>
@@ -5661,11 +5674,11 @@
       <c r="N80" s="4">
         <v>0</v>
       </c>
-      <c r="O80" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15">
+      <c r="O80" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>13</v>
       </c>
@@ -5673,269 +5686,269 @@
         <v>41961</v>
       </c>
       <c r="C81" s="3">
-        <v>0.27083333333333331</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="D81" s="3">
         <v>0.52430555555555558</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F81" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G81" s="4">
-        <v>0</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="H81" s="4">
-        <v>0</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="I81" s="4">
-        <v>0</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>25</v>
+        <v>0.01</v>
+      </c>
+      <c r="J81" s="4">
+        <v>0</v>
       </c>
       <c r="K81" s="4">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="L81" s="4">
-        <v>-0.73</v>
+        <v>-1.66</v>
       </c>
       <c r="M81" s="4">
         <v>0</v>
       </c>
       <c r="N81" s="4">
-        <v>0</v>
-      </c>
-      <c r="O81" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15">
+        <v>1</v>
+      </c>
+      <c r="O81" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B82" s="2">
-        <v>41961</v>
+        <v>41963</v>
       </c>
       <c r="C82" s="3">
-        <v>0.27083333333333331</v>
+        <v>0.42361111111111099</v>
       </c>
       <c r="D82" s="3">
-        <v>0.52430555555555558</v>
+        <v>0.46527777777777801</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F82" t="s">
+        <v>20</v>
+      </c>
+      <c r="G82" s="4">
+        <v>-4.0000000000000036E-3</v>
+      </c>
+      <c r="H82" s="4">
+        <v>-4.0000000000000036E-3</v>
+      </c>
+      <c r="I82" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J82" t="s">
+        <v>16</v>
+      </c>
+      <c r="K82" s="4">
+        <v>0</v>
+      </c>
+      <c r="L82" s="4">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="M82" s="4">
+        <v>0</v>
+      </c>
+      <c r="N82" s="4">
+        <v>0</v>
+      </c>
+      <c r="O82" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C83" s="3">
+        <v>0.42361111111111099</v>
+      </c>
+      <c r="D83" s="3">
+        <v>0.46527777777777801</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F83" t="s">
+        <v>19</v>
+      </c>
+      <c r="G83" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="H83" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="I83" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J83" t="s">
+        <v>16</v>
+      </c>
+      <c r="K83" s="4">
+        <v>0</v>
+      </c>
+      <c r="L83" s="4">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="M83" s="4">
+        <v>0</v>
+      </c>
+      <c r="N83" s="4">
+        <v>0</v>
+      </c>
+      <c r="O83" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B84" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C84" s="3">
+        <v>0.42361111111111099</v>
+      </c>
+      <c r="D84" s="3">
+        <v>0.46527777777777801</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F84" t="s">
+        <v>22</v>
+      </c>
+      <c r="G84" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="H84" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="I84" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J84" t="s">
         <v>26</v>
       </c>
-      <c r="G82" s="4">
-        <v>0</v>
-      </c>
-      <c r="H82" s="4">
-        <v>0</v>
-      </c>
-      <c r="I82" s="4">
-        <v>0</v>
-      </c>
-      <c r="J82" s="4" t="s">
+      <c r="K84" s="4">
+        <v>0</v>
+      </c>
+      <c r="L84" s="4">
+        <v>-0.66500000000000004</v>
+      </c>
+      <c r="M84" s="4">
+        <v>0</v>
+      </c>
+      <c r="N84" s="4">
+        <v>0</v>
+      </c>
+      <c r="O84" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B85" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C85" s="3">
+        <v>0.42361111111111099</v>
+      </c>
+      <c r="D85" s="3">
+        <v>0.46527777777777801</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F85" t="s">
+        <v>24</v>
+      </c>
+      <c r="G85" s="4">
+        <v>8.0999999999999989E-2</v>
+      </c>
+      <c r="H85" s="4">
+        <v>8.0999999999999989E-2</v>
+      </c>
+      <c r="I85" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J85" t="s">
         <v>26</v>
       </c>
-      <c r="K82" s="4">
-        <v>-0.05</v>
-      </c>
-      <c r="L82" s="4">
-        <v>-0.73</v>
-      </c>
-      <c r="M82" s="4">
-        <v>0</v>
-      </c>
-      <c r="N82" s="4">
-        <v>0</v>
-      </c>
-      <c r="O82" s="9" t="s">
+      <c r="K85" s="4">
+        <v>0</v>
+      </c>
+      <c r="L85" s="4">
+        <v>-0.92900000000000005</v>
+      </c>
+      <c r="M85" s="4">
+        <v>0</v>
+      </c>
+      <c r="N85" s="4">
+        <v>0</v>
+      </c>
+      <c r="O85" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B86" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C86" s="3">
+        <v>0.42361111111111099</v>
+      </c>
+      <c r="D86" s="3">
+        <v>0.46527777777777801</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F86" t="s">
+        <v>21</v>
+      </c>
+      <c r="G86" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="H86" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="I86" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J86" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="83" spans="1:15">
-      <c r="A83" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B83" s="2">
-        <v>41961</v>
-      </c>
-      <c r="C83" s="3">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="D83" s="3">
-        <v>0.52430555555555558</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F83" t="s">
-        <v>10</v>
-      </c>
-      <c r="G83" s="4">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="H83" s="4">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="I83" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J83" s="4">
-        <v>0</v>
-      </c>
-      <c r="K83" s="4">
-        <v>0</v>
-      </c>
-      <c r="L83" s="4">
-        <v>0</v>
-      </c>
-      <c r="M83" s="4">
-        <v>0</v>
-      </c>
-      <c r="N83" s="4">
-        <v>0</v>
-      </c>
-      <c r="O83" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15">
-      <c r="A84" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B84" s="2">
-        <v>41961</v>
-      </c>
-      <c r="C84" s="3">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="D84" s="3">
-        <v>0.47569444444444442</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F84" t="s">
-        <v>12</v>
-      </c>
-      <c r="G84" s="4">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="H84" s="4">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="I84" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J84" s="4">
-        <v>0</v>
-      </c>
-      <c r="K84" s="4">
-        <v>0</v>
-      </c>
-      <c r="L84" s="4">
-        <v>0</v>
-      </c>
-      <c r="M84" s="4">
-        <v>0</v>
-      </c>
-      <c r="N84" s="4">
-        <v>1</v>
-      </c>
-      <c r="O84" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15">
-      <c r="A85" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B85" s="2">
-        <v>41961</v>
-      </c>
-      <c r="C85" s="3">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="D85" s="3">
-        <v>0.52430555555555558</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F85" t="s">
-        <v>3</v>
-      </c>
-      <c r="G85" s="4">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="H85" s="4">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="I85" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J85" s="4">
-        <v>0</v>
-      </c>
-      <c r="K85" s="4">
-        <v>0</v>
-      </c>
-      <c r="L85" s="4">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="M85" s="4">
-        <v>0</v>
-      </c>
-      <c r="N85" s="4">
-        <v>0</v>
-      </c>
-      <c r="O85" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15">
-      <c r="A86" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B86" s="2">
-        <v>41961</v>
-      </c>
-      <c r="C86" s="3">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="D86" s="3">
-        <v>0.52430555555555558</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F86" t="s">
-        <v>11</v>
-      </c>
-      <c r="G86" s="4">
-        <v>1.7809999999999999</v>
-      </c>
-      <c r="H86" s="4">
-        <v>1.7809999999999999</v>
-      </c>
-      <c r="I86" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J86" s="4">
-        <v>0</v>
-      </c>
       <c r="K86" s="4">
         <v>0</v>
       </c>
       <c r="L86" s="4">
-        <v>-0.73</v>
+        <v>-0.496</v>
       </c>
       <c r="M86" s="4">
         <v>0</v>
@@ -5943,46 +5956,46 @@
       <c r="N86" s="4">
         <v>0</v>
       </c>
-      <c r="O86" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15">
+      <c r="O86" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B87" s="2">
-        <v>41961</v>
+        <v>41963</v>
       </c>
       <c r="C87" s="3">
-        <v>0.27083333333333331</v>
+        <v>0.42361111111111099</v>
       </c>
       <c r="D87" s="3">
-        <v>0.52430555555555558</v>
+        <v>0.46527777777777801</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F87" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G87" s="4">
-        <v>0</v>
+        <v>-9.7000000000000003E-2</v>
       </c>
       <c r="H87" s="4">
-        <v>0</v>
+        <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I87" s="4">
-        <v>0</v>
-      </c>
-      <c r="J87" s="4">
-        <v>0</v>
+        <v>1E-3</v>
+      </c>
+      <c r="J87" t="s">
+        <v>26</v>
       </c>
       <c r="K87" s="4">
         <v>0</v>
       </c>
       <c r="L87" s="4">
-        <v>0</v>
+        <v>-0.92900000000000005</v>
       </c>
       <c r="M87" s="4">
         <v>0</v>
@@ -5990,28 +6003,28 @@
       <c r="N87" s="4">
         <v>0</v>
       </c>
-      <c r="O87" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15">
+      <c r="O87" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B88" s="2">
-        <v>41961</v>
+        <v>41963</v>
       </c>
       <c r="C88" s="3">
-        <v>0.27083333333333331</v>
+        <v>0.42361111111111099</v>
       </c>
       <c r="D88" s="3">
-        <v>0.52430555555555558</v>
+        <v>0.46527777777777773</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F88" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G88" s="4">
         <v>-0.155</v>
@@ -6029,66 +6042,66 @@
         <v>0</v>
       </c>
       <c r="L88" s="4">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M88" s="4">
+        <v>0</v>
+      </c>
+      <c r="N88" s="4">
+        <v>0</v>
+      </c>
+      <c r="O88" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B89" s="2">
+        <v>41963</v>
+      </c>
+      <c r="C89" s="3">
+        <v>0.42361111111111099</v>
+      </c>
+      <c r="D89" s="3">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F89" t="s">
+        <v>17</v>
+      </c>
+      <c r="G89" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="H89" s="4">
+        <v>-0.155</v>
+      </c>
+      <c r="I89" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J89" t="s">
+        <v>16</v>
+      </c>
+      <c r="K89" s="4">
+        <v>0</v>
+      </c>
+      <c r="L89" s="4">
         <v>0.251</v>
       </c>
-      <c r="M88" s="4">
-        <v>0</v>
-      </c>
-      <c r="N88" s="4">
-        <v>0</v>
-      </c>
-      <c r="O88" s="8" t="s">
+      <c r="M89" s="4">
+        <v>0</v>
+      </c>
+      <c r="N89" s="4">
+        <v>0</v>
+      </c>
+      <c r="O89" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="89" spans="1:15">
-      <c r="A89" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B89" s="2">
-        <v>41961</v>
-      </c>
-      <c r="C89" s="3">
-        <v>0.4826388888888889</v>
-      </c>
-      <c r="D89" s="3">
-        <v>0.52430555555555558</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F89" t="s">
-        <v>12</v>
-      </c>
-      <c r="G89" s="4">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="H89" s="4">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="I89" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J89" s="4">
-        <v>0</v>
-      </c>
-      <c r="K89" s="4">
-        <v>0</v>
-      </c>
-      <c r="L89" s="4">
-        <v>-1.66</v>
-      </c>
-      <c r="M89" s="4">
-        <v>0</v>
-      </c>
-      <c r="N89" s="4">
-        <v>1</v>
-      </c>
-      <c r="O89" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>13</v>
       </c>
@@ -6096,34 +6109,34 @@
         <v>41963</v>
       </c>
       <c r="C90" s="3">
-        <v>0.42361111111111099</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D90" s="3">
-        <v>0.46527777777777801</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F90" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G90" s="4">
-        <v>-4.0000000000000036E-3</v>
+        <v>0</v>
       </c>
       <c r="H90" s="4">
-        <v>-4.0000000000000036E-3</v>
+        <v>0</v>
       </c>
       <c r="I90" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J90" t="s">
+        <v>0</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K90" s="4">
-        <v>0</v>
+      <c r="K90" s="5">
+        <v>-0.05</v>
       </c>
       <c r="L90" s="4">
-        <v>-7.9000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="M90" s="4">
         <v>0</v>
@@ -6132,10 +6145,10 @@
         <v>0</v>
       </c>
       <c r="O90" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>13</v>
       </c>
@@ -6143,34 +6156,34 @@
         <v>41963</v>
       </c>
       <c r="C91" s="3">
-        <v>0.42361111111111099</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D91" s="3">
-        <v>0.46527777777777801</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F91" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G91" s="4">
-        <v>-0.155</v>
+        <v>0</v>
       </c>
       <c r="H91" s="4">
-        <v>-0.155</v>
+        <v>0</v>
       </c>
       <c r="I91" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J91" t="s">
-        <v>16</v>
-      </c>
-      <c r="K91" s="4">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K91" s="5">
+        <v>-0.125</v>
       </c>
       <c r="L91" s="4">
-        <v>-7.9000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="M91" s="4">
         <v>0</v>
@@ -6179,10 +6192,10 @@
         <v>0</v>
       </c>
       <c r="O91" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>13</v>
       </c>
@@ -6190,34 +6203,34 @@
         <v>41963</v>
       </c>
       <c r="C92" s="3">
-        <v>0.42361111111111099</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D92" s="3">
-        <v>0.46527777777777801</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F92" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G92" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="H92" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="I92" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J92" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="K92" s="4">
-        <v>0</v>
-      </c>
-      <c r="L92" s="4">
-        <v>-0.66500000000000004</v>
+        <v>-0.2</v>
+      </c>
+      <c r="L92" s="5">
+        <v>-0.73</v>
       </c>
       <c r="M92" s="4">
         <v>0</v>
@@ -6225,11 +6238,11 @@
       <c r="N92" s="4">
         <v>0</v>
       </c>
-      <c r="O92" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15">
+      <c r="O92" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>13</v>
       </c>
@@ -6237,34 +6250,34 @@
         <v>41963</v>
       </c>
       <c r="C93" s="3">
-        <v>0.42361111111111099</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D93" s="3">
-        <v>0.46527777777777801</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F93" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G93" s="4">
-        <v>8.0999999999999989E-2</v>
+        <v>0</v>
       </c>
       <c r="H93" s="4">
-        <v>8.0999999999999989E-2</v>
+        <v>0</v>
       </c>
       <c r="I93" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J93" t="s">
+        <v>0</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>26</v>
       </c>
       <c r="K93" s="4">
-        <v>0</v>
-      </c>
-      <c r="L93" s="4">
-        <v>-0.92900000000000005</v>
+        <v>-0.05</v>
+      </c>
+      <c r="L93" s="5">
+        <v>-0.73</v>
       </c>
       <c r="M93" s="4">
         <v>0</v>
@@ -6272,11 +6285,11 @@
       <c r="N93" s="4">
         <v>0</v>
       </c>
-      <c r="O93" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15">
+      <c r="O93" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>13</v>
       </c>
@@ -6284,34 +6297,34 @@
         <v>41963</v>
       </c>
       <c r="C94" s="3">
-        <v>0.42361111111111099</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D94" s="3">
-        <v>0.46527777777777801</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F94" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G94" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>0.98099999999999998</v>
       </c>
       <c r="H94" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="I94" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J94" t="s">
-        <v>26</v>
+        <v>0.01</v>
+      </c>
+      <c r="J94" s="4">
+        <v>0</v>
       </c>
       <c r="K94" s="4">
         <v>0</v>
       </c>
       <c r="L94" s="4">
-        <v>-0.496</v>
+        <v>0</v>
       </c>
       <c r="M94" s="4">
         <v>0</v>
@@ -6319,11 +6332,11 @@
       <c r="N94" s="4">
         <v>0</v>
       </c>
-      <c r="O94" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15">
+      <c r="O94" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>13</v>
       </c>
@@ -6331,46 +6344,46 @@
         <v>41963</v>
       </c>
       <c r="C95" s="3">
-        <v>0.42361111111111099</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D95" s="3">
-        <v>0.46527777777777801</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F95" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G95" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>2.5950000000000002</v>
       </c>
       <c r="H95" s="4">
-        <v>-9.7000000000000003E-2</v>
+        <v>2.569</v>
       </c>
       <c r="I95" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J95" t="s">
-        <v>26</v>
+        <v>0.01</v>
+      </c>
+      <c r="J95" s="4">
+        <v>0</v>
       </c>
       <c r="K95" s="4">
         <v>0</v>
       </c>
       <c r="L95" s="4">
-        <v>-0.92900000000000005</v>
+        <v>0</v>
       </c>
       <c r="M95" s="4">
         <v>0</v>
       </c>
       <c r="N95" s="4">
-        <v>0</v>
-      </c>
-      <c r="O95" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15">
+        <v>1</v>
+      </c>
+      <c r="O95" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>13</v>
       </c>
@@ -6378,34 +6391,34 @@
         <v>41963</v>
       </c>
       <c r="C96" s="3">
-        <v>0.42361111111111099</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D96" s="3">
-        <v>0.46527777777777773</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F96" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G96" s="4">
-        <v>-0.155</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="H96" s="4">
-        <v>-0.155</v>
+        <v>0.46</v>
       </c>
       <c r="I96" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J96" t="s">
-        <v>16</v>
+        <v>0.01</v>
+      </c>
+      <c r="J96" s="4">
+        <v>0</v>
       </c>
       <c r="K96" s="4">
         <v>0</v>
       </c>
       <c r="L96" s="4">
-        <v>8.2000000000000003E-2</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="M96" s="4">
         <v>0</v>
@@ -6413,11 +6426,11 @@
       <c r="N96" s="4">
         <v>0</v>
       </c>
-      <c r="O96" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15">
+      <c r="O96" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>13</v>
       </c>
@@ -6425,34 +6438,34 @@
         <v>41963</v>
       </c>
       <c r="C97" s="3">
-        <v>0.42361111111111099</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D97" s="3">
-        <v>0.46527777777777773</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F97" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G97" s="4">
-        <v>-0.155</v>
+        <v>1.776</v>
       </c>
       <c r="H97" s="4">
-        <v>-0.155</v>
+        <v>1.7370000000000001</v>
       </c>
       <c r="I97" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J97" t="s">
-        <v>16</v>
+        <v>0.01</v>
+      </c>
+      <c r="J97" s="4">
+        <v>0</v>
       </c>
       <c r="K97" s="4">
         <v>0</v>
       </c>
       <c r="L97" s="4">
-        <v>0.251</v>
+        <v>-0.748</v>
       </c>
       <c r="M97" s="4">
         <v>0</v>
@@ -6460,11 +6473,11 @@
       <c r="N97" s="4">
         <v>0</v>
       </c>
-      <c r="O97" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15">
+      <c r="O97" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>13</v>
       </c>
@@ -6478,10 +6491,10 @@
         <v>0.51388888888888895</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G98" s="4">
         <v>0</v>
@@ -6492,11 +6505,11 @@
       <c r="I98" s="4">
         <v>0</v>
       </c>
-      <c r="J98" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K98" s="5">
-        <v>-0.05</v>
+      <c r="J98" s="4">
+        <v>0</v>
+      </c>
+      <c r="K98" s="4">
+        <v>0</v>
       </c>
       <c r="L98" s="4">
         <v>0</v>
@@ -6507,11 +6520,11 @@
       <c r="N98" s="4">
         <v>0</v>
       </c>
-      <c r="O98" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15">
+      <c r="O98" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>13</v>
       </c>
@@ -6519,46 +6532,46 @@
         <v>41963</v>
       </c>
       <c r="C99" s="3">
-        <v>0.4236111111111111</v>
+        <v>0.47222222222222199</v>
       </c>
       <c r="D99" s="3">
         <v>0.51388888888888895</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F99" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G99" s="4">
-        <v>0</v>
+        <v>-0.155</v>
       </c>
       <c r="H99" s="4">
-        <v>0</v>
+        <v>-0.155</v>
       </c>
       <c r="I99" s="4">
-        <v>0</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K99" s="5">
-        <v>-0.125</v>
+        <v>1E-3</v>
+      </c>
+      <c r="J99" t="s">
+        <v>16</v>
+      </c>
+      <c r="K99" s="4">
+        <v>0</v>
       </c>
       <c r="L99" s="4">
-        <v>0</v>
+        <v>-7.9000000000000001E-2</v>
       </c>
       <c r="M99" s="4">
         <v>0</v>
       </c>
       <c r="N99" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O99" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>13</v>
       </c>
@@ -6566,34 +6579,34 @@
         <v>41963</v>
       </c>
       <c r="C100" s="3">
-        <v>0.4236111111111111</v>
+        <v>0.47222222222222199</v>
       </c>
       <c r="D100" s="3">
         <v>0.51388888888888895</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F100" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G100" s="4">
-        <v>0</v>
+        <v>-4.0000000000000036E-3</v>
       </c>
       <c r="H100" s="4">
-        <v>0</v>
+        <v>-4.0000000000000036E-3</v>
       </c>
       <c r="I100" s="4">
-        <v>0</v>
-      </c>
-      <c r="J100" s="4" t="s">
-        <v>25</v>
+        <v>1E-3</v>
+      </c>
+      <c r="J100" t="s">
+        <v>16</v>
       </c>
       <c r="K100" s="4">
-        <v>-0.2</v>
-      </c>
-      <c r="L100" s="5">
-        <v>-0.73</v>
+        <v>0</v>
+      </c>
+      <c r="L100" s="4">
+        <v>-7.9000000000000001E-2</v>
       </c>
       <c r="M100" s="4">
         <v>0</v>
@@ -6601,11 +6614,11 @@
       <c r="N100" s="4">
         <v>0</v>
       </c>
-      <c r="O100" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15">
+      <c r="O100" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>13</v>
       </c>
@@ -6613,34 +6626,34 @@
         <v>41963</v>
       </c>
       <c r="C101" s="3">
-        <v>0.4236111111111111</v>
+        <v>0.47222222222222199</v>
       </c>
       <c r="D101" s="3">
         <v>0.51388888888888895</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F101" t="s">
+        <v>21</v>
+      </c>
+      <c r="G101" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="H101" s="4">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="I101" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="J101" t="s">
         <v>26</v>
       </c>
-      <c r="G101" s="4">
-        <v>0</v>
-      </c>
-      <c r="H101" s="4">
-        <v>0</v>
-      </c>
-      <c r="I101" s="4">
-        <v>0</v>
-      </c>
-      <c r="J101" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="K101" s="4">
-        <v>-0.05</v>
-      </c>
-      <c r="L101" s="5">
-        <v>-0.73</v>
+        <v>0</v>
+      </c>
+      <c r="L101" s="4">
+        <v>-0.496</v>
       </c>
       <c r="M101" s="4">
         <v>0</v>
@@ -6648,11 +6661,11 @@
       <c r="N101" s="4">
         <v>0</v>
       </c>
-      <c r="O101" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15">
+      <c r="O101" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>13</v>
       </c>
@@ -6660,34 +6673,34 @@
         <v>41963</v>
       </c>
       <c r="C102" s="3">
-        <v>0.4236111111111111</v>
+        <v>0.47222222222222199</v>
       </c>
       <c r="D102" s="3">
         <v>0.51388888888888895</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F102" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G102" s="4">
-        <v>0.98099999999999998</v>
+        <v>-9.7000000000000003E-2</v>
       </c>
       <c r="H102" s="4">
-        <v>0.95499999999999996</v>
+        <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I102" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J102" s="4">
-        <v>0</v>
+        <v>1E-3</v>
+      </c>
+      <c r="J102" t="s">
+        <v>26</v>
       </c>
       <c r="K102" s="4">
         <v>0</v>
       </c>
       <c r="L102" s="4">
-        <v>0</v>
+        <v>-0.66500000000000004</v>
       </c>
       <c r="M102" s="4">
         <v>0</v>
@@ -6695,11 +6708,11 @@
       <c r="N102" s="4">
         <v>0</v>
       </c>
-      <c r="O102" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15">
+      <c r="O102" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>13</v>
       </c>
@@ -6707,46 +6720,46 @@
         <v>41963</v>
       </c>
       <c r="C103" s="3">
-        <v>0.4236111111111111</v>
+        <v>0.47222222222222199</v>
       </c>
       <c r="D103" s="3">
         <v>0.51388888888888895</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F103" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G103" s="4">
-        <v>2.5950000000000002</v>
+        <v>-9.7000000000000003E-2</v>
       </c>
       <c r="H103" s="4">
-        <v>2.569</v>
+        <v>-9.7000000000000003E-2</v>
       </c>
       <c r="I103" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J103" s="4">
-        <v>0</v>
+        <v>1E-3</v>
+      </c>
+      <c r="J103" t="s">
+        <v>26</v>
       </c>
       <c r="K103" s="4">
         <v>0</v>
       </c>
       <c r="L103" s="4">
-        <v>0</v>
+        <v>-0.92900000000000005</v>
       </c>
       <c r="M103" s="4">
         <v>0</v>
       </c>
       <c r="N103" s="4">
-        <v>1</v>
-      </c>
-      <c r="O103" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15">
+        <v>0</v>
+      </c>
+      <c r="O103" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>13</v>
       </c>
@@ -6754,34 +6767,34 @@
         <v>41963</v>
       </c>
       <c r="C104" s="3">
-        <v>0.4236111111111111</v>
+        <v>0.47222222222222199</v>
       </c>
       <c r="D104" s="3">
         <v>0.51388888888888895</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F104" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G104" s="4">
-        <v>0.45400000000000001</v>
+        <v>8.0999999999999989E-2</v>
       </c>
       <c r="H104" s="4">
-        <v>0.46</v>
+        <v>8.0999999999999989E-2</v>
       </c>
       <c r="I104" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J104" s="4">
-        <v>0</v>
+        <v>1E-3</v>
+      </c>
+      <c r="J104" t="s">
+        <v>26</v>
       </c>
       <c r="K104" s="4">
         <v>0</v>
       </c>
       <c r="L104" s="4">
-        <v>0.97399999999999998</v>
+        <v>-0.92900000000000005</v>
       </c>
       <c r="M104" s="4">
         <v>0</v>
@@ -6789,11 +6802,11 @@
       <c r="N104" s="4">
         <v>0</v>
       </c>
-      <c r="O104" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15">
+      <c r="O104" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>13</v>
       </c>
@@ -6801,46 +6814,46 @@
         <v>41963</v>
       </c>
       <c r="C105" s="3">
-        <v>0.4236111111111111</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="D105" s="3">
         <v>0.51388888888888895</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F105" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G105" s="4">
-        <v>1.776</v>
+        <v>-0.155</v>
       </c>
       <c r="H105" s="4">
-        <v>1.7370000000000001</v>
+        <v>-0.155</v>
       </c>
       <c r="I105" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J105" s="4">
-        <v>0</v>
+        <v>1E-3</v>
+      </c>
+      <c r="J105" t="s">
+        <v>16</v>
       </c>
       <c r="K105" s="4">
         <v>0</v>
       </c>
       <c r="L105" s="4">
-        <v>-0.748</v>
+        <v>0.251</v>
       </c>
       <c r="M105" s="4">
         <v>0</v>
       </c>
       <c r="N105" s="4">
-        <v>0</v>
-      </c>
-      <c r="O105" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15">
+        <v>1</v>
+      </c>
+      <c r="O105" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>13</v>
       </c>
@@ -6848,418 +6861,42 @@
         <v>41963</v>
       </c>
       <c r="C106" s="3">
-        <v>0.4236111111111111</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="D106" s="3">
         <v>0.51388888888888895</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F106" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G106" s="4">
-        <v>0</v>
+        <v>-0.155</v>
       </c>
       <c r="H106" s="4">
-        <v>0</v>
+        <v>-0.155</v>
       </c>
       <c r="I106" s="4">
-        <v>0</v>
-      </c>
-      <c r="J106" s="4">
-        <v>0</v>
+        <v>1E-3</v>
+      </c>
+      <c r="J106" t="s">
+        <v>16</v>
       </c>
       <c r="K106" s="4">
         <v>0</v>
       </c>
       <c r="L106" s="4">
-        <v>0</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="M106" s="4">
         <v>0</v>
       </c>
       <c r="N106" s="4">
-        <v>0</v>
-      </c>
-      <c r="O106" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15">
-      <c r="A107" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B107" s="2">
-        <v>41963</v>
-      </c>
-      <c r="C107" s="3">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="D107" s="3">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F107" t="s">
-        <v>19</v>
-      </c>
-      <c r="G107" s="4">
-        <v>-0.155</v>
-      </c>
-      <c r="H107" s="4">
-        <v>-0.155</v>
-      </c>
-      <c r="I107" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J107" t="s">
-        <v>16</v>
-      </c>
-      <c r="K107" s="4">
-        <v>0</v>
-      </c>
-      <c r="L107" s="4">
-        <v>-7.9000000000000001E-2</v>
-      </c>
-      <c r="M107" s="4">
-        <v>0</v>
-      </c>
-      <c r="N107" s="4">
         <v>1</v>
       </c>
-      <c r="O107" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15">
-      <c r="A108" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B108" s="2">
-        <v>41963</v>
-      </c>
-      <c r="C108" s="3">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="D108" s="3">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F108" t="s">
-        <v>20</v>
-      </c>
-      <c r="G108" s="4">
-        <v>-4.0000000000000036E-3</v>
-      </c>
-      <c r="H108" s="4">
-        <v>-4.0000000000000036E-3</v>
-      </c>
-      <c r="I108" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J108" t="s">
-        <v>16</v>
-      </c>
-      <c r="K108" s="4">
-        <v>0</v>
-      </c>
-      <c r="L108" s="4">
-        <v>-7.9000000000000001E-2</v>
-      </c>
-      <c r="M108" s="4">
-        <v>0</v>
-      </c>
-      <c r="N108" s="4">
-        <v>0</v>
-      </c>
-      <c r="O108" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15">
-      <c r="A109" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B109" s="2">
-        <v>41963</v>
-      </c>
-      <c r="C109" s="3">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="D109" s="3">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F109" t="s">
-        <v>21</v>
-      </c>
-      <c r="G109" s="4">
-        <v>-9.7000000000000003E-2</v>
-      </c>
-      <c r="H109" s="4">
-        <v>-9.7000000000000003E-2</v>
-      </c>
-      <c r="I109" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J109" t="s">
-        <v>26</v>
-      </c>
-      <c r="K109" s="4">
-        <v>0</v>
-      </c>
-      <c r="L109" s="4">
-        <v>-0.496</v>
-      </c>
-      <c r="M109" s="4">
-        <v>0</v>
-      </c>
-      <c r="N109" s="4">
-        <v>0</v>
-      </c>
-      <c r="O109" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15">
-      <c r="A110" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B110" s="2">
-        <v>41963</v>
-      </c>
-      <c r="C110" s="3">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="D110" s="3">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F110" t="s">
-        <v>22</v>
-      </c>
-      <c r="G110" s="4">
-        <v>-9.7000000000000003E-2</v>
-      </c>
-      <c r="H110" s="4">
-        <v>-9.7000000000000003E-2</v>
-      </c>
-      <c r="I110" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J110" t="s">
-        <v>26</v>
-      </c>
-      <c r="K110" s="4">
-        <v>0</v>
-      </c>
-      <c r="L110" s="4">
-        <v>-0.66500000000000004</v>
-      </c>
-      <c r="M110" s="4">
-        <v>0</v>
-      </c>
-      <c r="N110" s="4">
-        <v>0</v>
-      </c>
-      <c r="O110" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15">
-      <c r="A111" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B111" s="2">
-        <v>41963</v>
-      </c>
-      <c r="C111" s="3">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="D111" s="3">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F111" t="s">
-        <v>23</v>
-      </c>
-      <c r="G111" s="4">
-        <v>-9.7000000000000003E-2</v>
-      </c>
-      <c r="H111" s="4">
-        <v>-9.7000000000000003E-2</v>
-      </c>
-      <c r="I111" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J111" t="s">
-        <v>26</v>
-      </c>
-      <c r="K111" s="4">
-        <v>0</v>
-      </c>
-      <c r="L111" s="4">
-        <v>-0.92900000000000005</v>
-      </c>
-      <c r="M111" s="4">
-        <v>0</v>
-      </c>
-      <c r="N111" s="4">
-        <v>0</v>
-      </c>
-      <c r="O111" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="112" spans="1:15">
-      <c r="A112" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B112" s="2">
-        <v>41963</v>
-      </c>
-      <c r="C112" s="3">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="D112" s="3">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F112" t="s">
-        <v>24</v>
-      </c>
-      <c r="G112" s="4">
-        <v>8.0999999999999989E-2</v>
-      </c>
-      <c r="H112" s="4">
-        <v>8.0999999999999989E-2</v>
-      </c>
-      <c r="I112" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J112" t="s">
-        <v>26</v>
-      </c>
-      <c r="K112" s="4">
-        <v>0</v>
-      </c>
-      <c r="L112" s="4">
-        <v>-0.92900000000000005</v>
-      </c>
-      <c r="M112" s="4">
-        <v>0</v>
-      </c>
-      <c r="N112" s="4">
-        <v>0</v>
-      </c>
-      <c r="O112" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15">
-      <c r="A113" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B113" s="2">
-        <v>41963</v>
-      </c>
-      <c r="C113" s="3">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="D113" s="3">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F113" t="s">
-        <v>17</v>
-      </c>
-      <c r="G113" s="4">
-        <v>-0.155</v>
-      </c>
-      <c r="H113" s="4">
-        <v>-0.155</v>
-      </c>
-      <c r="I113" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J113" t="s">
-        <v>16</v>
-      </c>
-      <c r="K113" s="4">
-        <v>0</v>
-      </c>
-      <c r="L113" s="4">
-        <v>0.251</v>
-      </c>
-      <c r="M113" s="4">
-        <v>0</v>
-      </c>
-      <c r="N113" s="4">
-        <v>1</v>
-      </c>
-      <c r="O113" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15">
-      <c r="A114" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B114" s="2">
-        <v>41963</v>
-      </c>
-      <c r="C114" s="3">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="D114" s="3">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F114" t="s">
-        <v>18</v>
-      </c>
-      <c r="G114" s="4">
-        <v>-0.155</v>
-      </c>
-      <c r="H114" s="4">
-        <v>-0.155</v>
-      </c>
-      <c r="I114" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="J114" t="s">
-        <v>16</v>
-      </c>
-      <c r="K114" s="4">
-        <v>0</v>
-      </c>
-      <c r="L114" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="M114" s="4">
-        <v>0</v>
-      </c>
-      <c r="N114" s="4">
-        <v>1</v>
-      </c>
-      <c r="O114" s="8" t="s">
+      <c r="O106" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -7272,10 +6909,5 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>